<commit_message>
remove data from data file
</commit_message>
<xml_diff>
--- a/tools/data.xlsx
+++ b/tools/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Playground\luckydraw\luckydraw\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PlayGround\Python\lucky_slot_separator\luckydraw\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B307D5AA-4801-4358-A168-695E31912AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74110668-936A-4B25-94A8-FF55AD8B76CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7260" yWindow="615" windowWidth="20730" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8205" yWindow="615" windowWidth="20730" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
@@ -20,21 +20,11 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="96">
   <si>
     <t>active</t>
   </si>
@@ -321,310 +311,7 @@
     <t>023570</t>
   </si>
   <si>
-    <t>Nguyễn Văn Dương</t>
-  </si>
-  <si>
-    <t>Nguyễn Nhật Bảo</t>
-  </si>
-  <si>
-    <t>Quách Thị Mỹ Linh</t>
-  </si>
-  <si>
-    <t>Trần Đăng Xuân</t>
-  </si>
-  <si>
-    <t>Nguyễn Nhật Linh</t>
-  </si>
-  <si>
-    <t>Trương Minh Hoàng</t>
-  </si>
-  <si>
-    <t>Phan Văn Hậu</t>
-  </si>
-  <si>
-    <t>Trương Quang Trường</t>
-  </si>
-  <si>
-    <t>Hoàng Nguyễn Hoài Nam</t>
-  </si>
-  <si>
-    <t>Phan Tấn Thái Dương</t>
-  </si>
-  <si>
-    <t>Phạm Bá Phúc</t>
-  </si>
-  <si>
-    <t>Trương Anh Hào</t>
-  </si>
-  <si>
-    <t>Đặng Minh Thiện</t>
-  </si>
-  <si>
-    <t>Nguyễn Minh Quang</t>
-  </si>
-  <si>
-    <t>Mai Thanh Mẫn</t>
-  </si>
-  <si>
-    <t>Phạm Thanh Tú</t>
-  </si>
-  <si>
-    <t>Lê Thị Ngọc Xuân</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Huyền Trang</t>
-  </si>
-  <si>
-    <t>Vũ Xuân Thắng</t>
-  </si>
-  <si>
-    <t>Trần Thị Ngọc Minh</t>
-  </si>
-  <si>
-    <t>Hoàng Hữu Đạt</t>
-  </si>
-  <si>
-    <t>Nguyễn Hữu Trọng</t>
-  </si>
-  <si>
-    <t>Hoàng Gia Vương</t>
-  </si>
-  <si>
-    <t>Kiều Văn Tiến</t>
-  </si>
-  <si>
-    <t>Trương Minh Đông</t>
-  </si>
-  <si>
-    <t>Thái Hoàng Đăng</t>
-  </si>
-  <si>
-    <t>Võ Tuấn Kiệt</t>
-  </si>
-  <si>
-    <t>Trần Doãn Tùng</t>
-  </si>
-  <si>
-    <t>Phan Thanh Hậu</t>
-  </si>
-  <si>
-    <t>Nguyễn Đoàn Thiên Thương</t>
-  </si>
-  <si>
-    <t>Thống A Thảo</t>
-  </si>
-  <si>
-    <t>Nguyễn Thanh Hoài</t>
-  </si>
-  <si>
-    <t>Đặng Vĩnh Trường</t>
-  </si>
-  <si>
-    <t>Nguyễn Việt Bắc</t>
-  </si>
-  <si>
-    <t>Nguyễn Thế Anh</t>
-  </si>
-  <si>
-    <t>Trần Huỳnh Tới</t>
-  </si>
-  <si>
-    <t>Bùi Xuân Trường</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Thu Hương</t>
-  </si>
-  <si>
-    <t>Trần Xuân Bình</t>
-  </si>
-  <si>
-    <t>Huỳnh Đại Nghĩa</t>
-  </si>
-  <si>
-    <t>Huỳnh Phạm Nhất Triều</t>
-  </si>
-  <si>
-    <t>Nguyễn Ngọc Lâm</t>
-  </si>
-  <si>
-    <t>Nguyễn Thanh Tùng</t>
-  </si>
-  <si>
-    <t>Trương Ngọc Nhất</t>
-  </si>
-  <si>
-    <t>Huỳnh Hiếu Nghĩa</t>
-  </si>
-  <si>
-    <t>Võ Quang Nhân</t>
-  </si>
-  <si>
-    <t>Ôn Quân An</t>
-  </si>
-  <si>
-    <t>Trà Anh Toàn</t>
-  </si>
-  <si>
-    <t>Trần Phúc Nguyên</t>
-  </si>
-  <si>
-    <t>Phan Đình Khang</t>
-  </si>
-  <si>
-    <t>Bùi Huỳnh Hạo Thiên</t>
-  </si>
-  <si>
-    <t>Trịnh Văn Hoàng</t>
-  </si>
-  <si>
-    <t>Đặng Huỳnh Song Thảo</t>
-  </si>
-  <si>
-    <t>Đỗ Thị Bích Trâm</t>
-  </si>
-  <si>
-    <t>Phan Lý Nhung</t>
-  </si>
-  <si>
-    <t>Trịnh Thị Minh</t>
-  </si>
-  <si>
-    <t>Nguyễn Duy Kha</t>
-  </si>
-  <si>
-    <t>Nguyễn Gia Bảo</t>
-  </si>
-  <si>
-    <t>Bùi Ngọc Bảo Trâm</t>
-  </si>
-  <si>
-    <t>Dương Nam</t>
-  </si>
-  <si>
-    <t>Lâm Chí Hiền</t>
-  </si>
-  <si>
-    <t>Từ Vương Bảo Ngọc</t>
-  </si>
-  <si>
-    <t>Lê Khắc Hoàn Vũ</t>
-  </si>
-  <si>
-    <t>Lê Việt Hoàng</t>
-  </si>
-  <si>
-    <t>Vũ Đình Cao</t>
-  </si>
-  <si>
-    <t>Đặng Hoàng Trọng</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn Thịnh</t>
-  </si>
-  <si>
-    <t>Phạm Xuân Quang</t>
-  </si>
-  <si>
-    <t>Đinh Anh Trung</t>
-  </si>
-  <si>
-    <t>Đặng Văn Anh Nguyên</t>
-  </si>
-  <si>
-    <t>Đỗ Diệu Trinh</t>
-  </si>
-  <si>
-    <t>Huỳnh Văn Hậu</t>
-  </si>
-  <si>
-    <t>Trần Minh Thiện</t>
-  </si>
-  <si>
-    <t>Đặng Thái Hiên</t>
-  </si>
-  <si>
-    <t>Võ Kim Thạch</t>
-  </si>
-  <si>
-    <t>Nguyễn Quang Thắng</t>
-  </si>
-  <si>
-    <t>Nguyễn Phan Thiện Long</t>
-  </si>
-  <si>
-    <t>Lê Minh Tuấn</t>
-  </si>
-  <si>
-    <t>Nguyễn Gia Huy</t>
-  </si>
-  <si>
-    <t>Võ Bình An</t>
-  </si>
-  <si>
-    <t>Võ Thị Kim Ngân</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn Hợp</t>
-  </si>
-  <si>
-    <t>Nguyễn Quang Chiến</t>
-  </si>
-  <si>
-    <t>Mai Dương Quyền</t>
-  </si>
-  <si>
-    <t>Nguyễn Duy Đăng</t>
-  </si>
-  <si>
-    <t>Phan Lê Thanh Tùng</t>
-  </si>
-  <si>
-    <t>Nguyễn Tuấn Khanh</t>
-  </si>
-  <si>
-    <t>Phạm Thanh Hải</t>
-  </si>
-  <si>
-    <t>Thái Tân Xuyên</t>
-  </si>
-  <si>
-    <t>Đặng Trần Tuấn</t>
-  </si>
-  <si>
-    <t>Đặng Ngàn Nhất Phương</t>
-  </si>
-  <si>
-    <t>Mai Hồng Thức</t>
-  </si>
-  <si>
-    <t>Trần Quang Thái</t>
-  </si>
-  <si>
-    <t>Đặng Nguyễn Nguyên Vũ</t>
-  </si>
-  <si>
-    <t>Đỗ Quang Vinh</t>
-  </si>
-  <si>
-    <t>Hoàng Quốc Vũ</t>
-  </si>
-  <si>
-    <t>Trần Gia Huấn</t>
-  </si>
-  <si>
-    <t>Thái Phạm Văn Hiệp</t>
-  </si>
-  <si>
-    <t>Trương Hoàng Lĩnh</t>
-  </si>
-  <si>
-    <t>Đỗ Duy Tân</t>
-  </si>
-  <si>
-    <t>Đặng Minh Nhật</t>
-  </si>
-  <si>
-    <t>Nguyễn Minh Cầm</t>
+    <t>Nguyễn Văn A</t>
   </si>
 </sst>
 </file>
@@ -761,7 +448,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[data_2.xlsx]Sheet2!PivotTable4</c:name>
+    <c:name>[data.xlsx]Sheet2!PivotTable4</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -910,47 +597,6 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="9"/>
@@ -967,47 +613,6 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="10"/>
@@ -1024,47 +629,6 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="11"/>
@@ -1081,47 +645,6 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="12"/>
@@ -1138,47 +661,6 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="13"/>
@@ -4263,7 +3745,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{94B01B55-908F-407E-A0F5-1EADA3A17688}" name="Table13" displayName="Table13" ref="A1:F103" totalsRowShown="0">
   <autoFilter ref="A1:F103" xr:uid="{28E80E7D-EF45-41A0-A381-C2279AEF5075}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F103">
+  <sortState ref="A2:F103">
     <sortCondition ref="E2:E103"/>
     <sortCondition ref="C2:C103"/>
   </sortState>
@@ -4602,8 +4084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4714BE-5015-4D45-92D9-EFF28A4D2C9F}">
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4658,7 +4140,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -4676,7 +4158,7 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -4694,7 +4176,7 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -4712,7 +4194,7 @@
         <v>197739</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -4730,7 +4212,7 @@
         <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -4748,7 +4230,7 @@
         <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -4766,7 +4248,7 @@
         <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -4784,7 +4266,7 @@
         <v>186265</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
@@ -4802,7 +4284,7 @@
         <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
@@ -4820,7 +4302,7 @@
         <v>197557</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
@@ -4838,7 +4320,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C13" s="1">
         <v>4</v>
@@ -4856,7 +4338,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C14" s="1">
         <v>4</v>
@@ -4874,7 +4356,7 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C15" s="1">
         <v>4</v>
@@ -4892,7 +4374,7 @@
         <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C16" s="1">
         <v>4</v>
@@ -4910,7 +4392,7 @@
         <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C17" s="1">
         <v>5</v>
@@ -4928,7 +4410,7 @@
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -4946,7 +4428,7 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C19" s="1">
         <v>5</v>
@@ -4964,7 +4446,7 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="C20" s="1">
         <v>5</v>
@@ -4982,7 +4464,7 @@
         <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="C21" s="1">
         <v>6</v>
@@ -5000,7 +4482,7 @@
         <v>197510</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C22" s="1">
         <v>7</v>
@@ -5018,7 +4500,7 @@
         <v>197734</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="C23" s="1">
         <v>7</v>
@@ -5036,7 +4518,7 @@
         <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="C24" s="1">
         <v>7</v>
@@ -5054,7 +4536,7 @@
         <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="C25" s="1">
         <v>7</v>
@@ -5072,7 +4554,7 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="C26" s="1">
         <v>7</v>
@@ -5090,7 +4572,7 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="C27" s="1">
         <v>8</v>
@@ -5108,7 +4590,7 @@
         <v>186824</v>
       </c>
       <c r="B28" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="C28" s="1">
         <v>8</v>
@@ -5126,7 +4608,7 @@
         <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
@@ -5144,7 +4626,7 @@
         <v>220175</v>
       </c>
       <c r="B30" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -5162,7 +4644,7 @@
         <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
@@ -5180,7 +4662,7 @@
         <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
@@ -5198,7 +4680,7 @@
         <v>220980</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
@@ -5216,7 +4698,7 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
@@ -5234,7 +4716,7 @@
         <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
@@ -5252,7 +4734,7 @@
         <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
@@ -5270,7 +4752,7 @@
         <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
@@ -5288,7 +4770,7 @@
         <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="C38" s="1">
         <v>2</v>
@@ -5306,7 +4788,7 @@
         <v>14</v>
       </c>
       <c r="B39" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="C39" s="1">
         <v>2</v>
@@ -5324,7 +4806,7 @@
         <v>208158</v>
       </c>
       <c r="B40" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="C40" s="1">
         <v>2</v>
@@ -5342,7 +4824,7 @@
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>134</v>
+        <v>95</v>
       </c>
       <c r="C41" s="1">
         <v>2</v>
@@ -5360,7 +4842,7 @@
         <v>68</v>
       </c>
       <c r="B42" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
       <c r="C42" s="1">
         <v>3</v>
@@ -5378,7 +4860,7 @@
         <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
       <c r="C43" s="1">
         <v>3</v>
@@ -5396,7 +4878,7 @@
         <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>95</v>
       </c>
       <c r="C44" s="1">
         <v>3</v>
@@ -5414,7 +4896,7 @@
         <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="C45" s="1">
         <v>3</v>
@@ -5432,7 +4914,7 @@
         <v>197299</v>
       </c>
       <c r="B46" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="C46" s="1">
         <v>3</v>
@@ -5450,7 +4932,7 @@
         <v>208351</v>
       </c>
       <c r="B47" t="s">
-        <v>140</v>
+        <v>95</v>
       </c>
       <c r="C47" s="1">
         <v>3</v>
@@ -5468,7 +4950,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="C48" s="1">
         <v>4</v>
@@ -5486,7 +4968,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="C49" s="1">
         <v>4</v>
@@ -5504,7 +4986,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>143</v>
+        <v>95</v>
       </c>
       <c r="C50" s="1">
         <v>4</v>
@@ -5522,7 +5004,7 @@
         <v>32</v>
       </c>
       <c r="B51" t="s">
-        <v>144</v>
+        <v>95</v>
       </c>
       <c r="C51" s="1">
         <v>4</v>
@@ -5540,7 +5022,7 @@
         <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="C52" s="1">
         <v>5</v>
@@ -5558,7 +5040,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
       <c r="C53" s="1">
         <v>5</v>
@@ -5576,7 +5058,7 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="C54" s="1">
         <v>5</v>
@@ -5594,7 +5076,7 @@
         <v>60</v>
       </c>
       <c r="B55" t="s">
-        <v>148</v>
+        <v>95</v>
       </c>
       <c r="C55" s="1">
         <v>5</v>
@@ -5612,7 +5094,7 @@
         <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>149</v>
+        <v>95</v>
       </c>
       <c r="C56" s="1">
         <v>5</v>
@@ -5630,7 +5112,7 @@
         <v>186745</v>
       </c>
       <c r="B57" t="s">
-        <v>150</v>
+        <v>95</v>
       </c>
       <c r="C57" s="1">
         <v>5</v>
@@ -5648,7 +5130,7 @@
         <v>45</v>
       </c>
       <c r="B58" t="s">
-        <v>151</v>
+        <v>95</v>
       </c>
       <c r="C58" s="1">
         <v>6</v>
@@ -5666,7 +5148,7 @@
         <v>52</v>
       </c>
       <c r="B59" t="s">
-        <v>152</v>
+        <v>95</v>
       </c>
       <c r="C59" s="1">
         <v>6</v>
@@ -5684,7 +5166,7 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>153</v>
+        <v>95</v>
       </c>
       <c r="C60" s="1">
         <v>6</v>
@@ -5702,7 +5184,7 @@
         <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>154</v>
+        <v>95</v>
       </c>
       <c r="C61" s="1">
         <v>6</v>
@@ -5720,7 +5202,7 @@
         <v>81</v>
       </c>
       <c r="B62" t="s">
-        <v>155</v>
+        <v>95</v>
       </c>
       <c r="C62" s="1">
         <v>6</v>
@@ -5738,7 +5220,7 @@
         <v>29</v>
       </c>
       <c r="B63" t="s">
-        <v>156</v>
+        <v>95</v>
       </c>
       <c r="C63" s="1">
         <v>6</v>
@@ -5756,7 +5238,7 @@
         <v>84</v>
       </c>
       <c r="B64" t="s">
-        <v>157</v>
+        <v>95</v>
       </c>
       <c r="C64" s="1">
         <v>6</v>
@@ -5774,7 +5256,7 @@
         <v>69</v>
       </c>
       <c r="B65" t="s">
-        <v>158</v>
+        <v>95</v>
       </c>
       <c r="C65" s="1">
         <v>7</v>
@@ -5792,7 +5274,7 @@
         <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
       <c r="C66" s="1">
         <v>7</v>
@@ -5810,7 +5292,7 @@
         <v>220986</v>
       </c>
       <c r="B67" t="s">
-        <v>160</v>
+        <v>95</v>
       </c>
       <c r="C67" s="1">
         <v>7</v>
@@ -5828,7 +5310,7 @@
         <v>74</v>
       </c>
       <c r="B68" t="s">
-        <v>161</v>
+        <v>95</v>
       </c>
       <c r="C68" s="1">
         <v>7</v>
@@ -5846,7 +5328,7 @@
         <v>75</v>
       </c>
       <c r="B69" t="s">
-        <v>162</v>
+        <v>95</v>
       </c>
       <c r="C69" s="1">
         <v>7</v>
@@ -5864,7 +5346,7 @@
         <v>78</v>
       </c>
       <c r="B70" t="s">
-        <v>163</v>
+        <v>95</v>
       </c>
       <c r="C70" s="1">
         <v>7</v>
@@ -5882,7 +5364,7 @@
         <v>94</v>
       </c>
       <c r="B71" t="s">
-        <v>164</v>
+        <v>95</v>
       </c>
       <c r="C71" s="1">
         <v>7</v>
@@ -5900,7 +5382,7 @@
         <v>87</v>
       </c>
       <c r="B72" t="s">
-        <v>165</v>
+        <v>95</v>
       </c>
       <c r="C72" s="1">
         <v>7</v>
@@ -5918,7 +5400,7 @@
         <v>38</v>
       </c>
       <c r="B73" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
       <c r="C73" s="1">
         <v>7</v>
@@ -5936,7 +5418,7 @@
         <v>47</v>
       </c>
       <c r="B74" t="s">
-        <v>167</v>
+        <v>95</v>
       </c>
       <c r="C74" s="1">
         <v>7</v>
@@ -5954,7 +5436,7 @@
         <v>59</v>
       </c>
       <c r="B75" t="s">
-        <v>168</v>
+        <v>95</v>
       </c>
       <c r="C75" s="1">
         <v>8</v>
@@ -5972,7 +5454,7 @@
         <v>61</v>
       </c>
       <c r="B76" t="s">
-        <v>169</v>
+        <v>95</v>
       </c>
       <c r="C76" s="1">
         <v>8</v>
@@ -5990,7 +5472,7 @@
         <v>65</v>
       </c>
       <c r="B77" t="s">
-        <v>170</v>
+        <v>95</v>
       </c>
       <c r="C77" s="1">
         <v>8</v>
@@ -6008,7 +5490,7 @@
         <v>67</v>
       </c>
       <c r="B78" t="s">
-        <v>171</v>
+        <v>95</v>
       </c>
       <c r="C78" s="1">
         <v>8</v>
@@ -6026,7 +5508,7 @@
         <v>71</v>
       </c>
       <c r="B79" t="s">
-        <v>172</v>
+        <v>95</v>
       </c>
       <c r="C79" s="1">
         <v>8</v>
@@ -6044,7 +5526,7 @@
         <v>72</v>
       </c>
       <c r="B80" t="s">
-        <v>173</v>
+        <v>95</v>
       </c>
       <c r="C80" s="1">
         <v>8</v>
@@ -6062,7 +5544,7 @@
         <v>73</v>
       </c>
       <c r="B81" t="s">
-        <v>174</v>
+        <v>95</v>
       </c>
       <c r="C81" s="1">
         <v>8</v>
@@ -6080,7 +5562,7 @@
         <v>79</v>
       </c>
       <c r="B82" t="s">
-        <v>175</v>
+        <v>95</v>
       </c>
       <c r="C82" s="1">
         <v>8</v>
@@ -6098,7 +5580,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>176</v>
+        <v>95</v>
       </c>
       <c r="C83" s="1">
         <v>8</v>
@@ -6116,7 +5598,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>177</v>
+        <v>95</v>
       </c>
       <c r="C84" s="1">
         <v>8</v>
@@ -6134,7 +5616,7 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>178</v>
+        <v>95</v>
       </c>
       <c r="C85" s="1">
         <v>8</v>
@@ -6152,7 +5634,7 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>179</v>
+        <v>95</v>
       </c>
       <c r="C86" s="1">
         <v>8</v>
@@ -6170,7 +5652,7 @@
         <v>24</v>
       </c>
       <c r="B87" t="s">
-        <v>180</v>
+        <v>95</v>
       </c>
       <c r="C87" s="1">
         <v>1</v>
@@ -6190,7 +5672,7 @@
         <v>231801</v>
       </c>
       <c r="B88" t="s">
-        <v>181</v>
+        <v>95</v>
       </c>
       <c r="C88" s="1">
         <v>1</v>
@@ -6210,7 +5692,7 @@
         <v>21</v>
       </c>
       <c r="B89" t="s">
-        <v>182</v>
+        <v>95</v>
       </c>
       <c r="C89" s="1">
         <v>2</v>
@@ -6230,7 +5712,7 @@
         <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="C90" s="1">
         <v>3</v>
@@ -6250,7 +5732,7 @@
         <v>8</v>
       </c>
       <c r="B91" t="s">
-        <v>184</v>
+        <v>95</v>
       </c>
       <c r="C91" s="1">
         <v>3</v>
@@ -6270,7 +5752,7 @@
         <v>11</v>
       </c>
       <c r="B92" t="s">
-        <v>185</v>
+        <v>95</v>
       </c>
       <c r="C92" s="1">
         <v>4</v>
@@ -6290,7 +5772,7 @@
         <v>12</v>
       </c>
       <c r="B93" t="s">
-        <v>186</v>
+        <v>95</v>
       </c>
       <c r="C93" s="1">
         <v>5</v>
@@ -6310,7 +5792,7 @@
         <v>17</v>
       </c>
       <c r="B94" t="s">
-        <v>187</v>
+        <v>95</v>
       </c>
       <c r="C94" s="1">
         <v>5</v>
@@ -6330,7 +5812,7 @@
         <v>13</v>
       </c>
       <c r="B95" t="s">
-        <v>188</v>
+        <v>95</v>
       </c>
       <c r="C95" s="1">
         <v>6</v>
@@ -6350,7 +5832,7 @@
         <v>76</v>
       </c>
       <c r="B96" t="s">
-        <v>189</v>
+        <v>95</v>
       </c>
       <c r="C96" s="1">
         <v>7</v>
@@ -6370,7 +5852,7 @@
         <v>10</v>
       </c>
       <c r="B97" t="s">
-        <v>190</v>
+        <v>95</v>
       </c>
       <c r="C97" s="1">
         <v>1</v>
@@ -6390,7 +5872,7 @@
         <v>5</v>
       </c>
       <c r="B98" t="s">
-        <v>191</v>
+        <v>95</v>
       </c>
       <c r="C98" s="1">
         <v>2</v>
@@ -6410,7 +5892,7 @@
         <v>980013</v>
       </c>
       <c r="B99" t="s">
-        <v>192</v>
+        <v>95</v>
       </c>
       <c r="C99" s="1">
         <v>1</v>
@@ -6430,7 +5912,7 @@
         <v>4</v>
       </c>
       <c r="B100" t="s">
-        <v>193</v>
+        <v>95</v>
       </c>
       <c r="C100" s="1">
         <v>1</v>
@@ -6450,7 +5932,7 @@
         <v>221296</v>
       </c>
       <c r="B101" t="s">
-        <v>194</v>
+        <v>95</v>
       </c>
       <c r="C101" s="1">
         <v>1</v>
@@ -6470,7 +5952,7 @@
         <v>7</v>
       </c>
       <c r="B102" t="s">
-        <v>195</v>
+        <v>95</v>
       </c>
       <c r="C102" s="1">
         <v>3</v>
@@ -6490,7 +5972,7 @@
         <v>186559</v>
       </c>
       <c r="B103" t="s">
-        <v>196</v>
+        <v>95</v>
       </c>
       <c r="C103" s="1">
         <v>8</v>

</xml_diff>